<commit_message>
create courses, topics, lessons, lms
</commit_message>
<xml_diff>
--- a/Test files/test.xlsx
+++ b/Test files/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\lms\Test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F01CE1-6765-4924-B620-C05D2899D14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45326D79-834F-46FF-8848-165AF0280629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3450" windowWidth="21570" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>câu hỏi</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>3c</t>
-  </si>
-  <si>
-    <t>3d</t>
   </si>
 </sst>
 </file>
@@ -411,7 +408,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,9 +495,6 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>